<commit_message>
First reading in 1
</commit_message>
<xml_diff>
--- a/Papers_QSCOUT.xlsx
+++ b/Papers_QSCOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jeonghyun\GIT\QSCOUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FF984E-286E-4231-B4CD-317454CE6CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E78CBBF-96CE-4161-9100-A8FD0AE699A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="4550" windowWidth="23170" windowHeight="11260" xr2:uid="{5AB8A0E6-92A3-4400-A3A6-B98A5E706936}"/>
+    <workbookView xWindow="0" yWindow="4140" windowWidth="23170" windowHeight="11260" xr2:uid="{5AB8A0E6-92A3-4400-A3A6-B98A5E706936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>C:\Jeonghyun\GIT\QSCOUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +80,20 @@
   </si>
   <si>
     <t>C:\Jeonghyun\GIT\QSCOUT\QASM</t>
+  </si>
+  <si>
+    <t>8_Gate Set Tomography</t>
+  </si>
+  <si>
+    <t>C:\Jeonghyun\GIT\QSCOUT\Gate_Set_Tomography</t>
+  </si>
+  <si>
+    <t>9_Determination of Multi-mode Motional Quantum States in a Trapped Ion System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10_Characterizing and mitigating coherent errors in a trapped ion quantum processor using hidden inverses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -443,16 +457,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8C3D5A-D15D-4E31-8E0A-7F7CAF893C4D}">
-  <dimension ref="C3:E10"/>
+  <dimension ref="C3:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="79.9140625" customWidth="1"/>
-    <col min="5" max="5" width="32.4140625" customWidth="1"/>
+    <col min="4" max="4" width="92.4140625" customWidth="1"/>
+    <col min="5" max="5" width="49.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.45">
@@ -543,6 +557,39 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new paper and reading
</commit_message>
<xml_diff>
--- a/Papers_QSCOUT.xlsx
+++ b/Papers_QSCOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jeonghyun\GIT\QSCOUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E78CBBF-96CE-4161-9100-A8FD0AE699A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0DB521-851C-4ED2-B0BA-1AFFCA005706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4140" windowWidth="23170" windowHeight="11260" xr2:uid="{5AB8A0E6-92A3-4400-A3A6-B98A5E706936}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>C:\Jeonghyun\GIT\QSCOUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,10 @@
   </si>
   <si>
     <t>10_Characterizing and mitigating coherent errors in a trapped ion quantum processor using hidden inverses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11_Improving Circuit Performance in a Trapped-Ion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -457,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8C3D5A-D15D-4E31-8E0A-7F7CAF893C4D}">
-  <dimension ref="C3:E13"/>
+  <dimension ref="C3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -590,6 +594,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New Qscout arch paper
</commit_message>
<xml_diff>
--- a/Papers_QSCOUT.xlsx
+++ b/Papers_QSCOUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jeonghyun\GIT\QSCOUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RFSoC\GIT\QSCOUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90A9B19-35EC-4972-B110-0E04657D85EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBC973-5533-4A0C-AA4E-13198403384C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="1760" windowWidth="15030" windowHeight="11260" xr2:uid="{5AB8A0E6-92A3-4400-A3A6-B98A5E706936}"/>
+    <workbookView xWindow="870" yWindow="1755" windowWidth="15030" windowHeight="11265" xr2:uid="{5AB8A0E6-92A3-4400-A3A6-B98A5E706936}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -23,23 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>C:\Jeonghyun\GIT\QSCOUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,6 +270,12 @@
   </si>
   <si>
     <t>C:\Jeonghyun\GIT\QSCOUT\CrossTalk</t>
+  </si>
+  <si>
+    <t>23_Efficient Z-Gates for Quantum Computing</t>
+  </si>
+  <si>
+    <t>24_Arbitrary_Waveform_Generator_for_Quantum_Informati</t>
   </si>
 </sst>
 </file>
@@ -644,20 +639,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8C3D5A-D15D-4E31-8E0A-7F7CAF893C4D}">
-  <dimension ref="C3:E25"/>
+  <dimension ref="C3:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="4" max="4" width="92.4140625" customWidth="1"/>
+    <col min="4" max="4" width="92.375" customWidth="1"/>
     <col min="5" max="5" width="49.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -668,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>1</v>
       </c>
@@ -679,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2</v>
       </c>
@@ -690,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>3</v>
       </c>
@@ -701,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>4</v>
       </c>
@@ -712,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>5</v>
       </c>
@@ -723,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>6</v>
       </c>
@@ -734,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>7</v>
       </c>
@@ -745,7 +740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>8</v>
       </c>
@@ -756,7 +751,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>9</v>
       </c>
@@ -767,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>10</v>
       </c>
@@ -778,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>11</v>
       </c>
@@ -789,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>12</v>
       </c>
@@ -800,7 +795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>13</v>
       </c>
@@ -811,7 +806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>14</v>
       </c>
@@ -822,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>15</v>
       </c>
@@ -833,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>16</v>
       </c>
@@ -844,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>17</v>
       </c>
@@ -855,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>18</v>
       </c>
@@ -866,7 +861,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>19</v>
       </c>
@@ -877,7 +872,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>20</v>
       </c>
@@ -888,7 +883,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>21</v>
       </c>
@@ -899,7 +894,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>22</v>
       </c>
@@ -908,11 +903,28 @@
       </c>
       <c r="E25" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -924,14 +936,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="92.4140625" customWidth="1"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="4" max="4" width="92.375" customWidth="1"/>
     <col min="5" max="5" width="49.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -942,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>21</v>
       </c>
@@ -953,7 +965,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>31</v>
       </c>
@@ -964,7 +976,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>30</v>
       </c>
@@ -975,7 +987,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>24</v>
       </c>
@@ -986,7 +998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -997,7 +1009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>33</v>
       </c>
@@ -1011,7 +1023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>35</v>
       </c>
@@ -1025,7 +1037,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>46</v>
       </c>
@@ -1039,7 +1051,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>48</v>
       </c>
@@ -1050,7 +1062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>51</v>
       </c>
@@ -1078,14 +1090,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="92.4140625" customWidth="1"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="4" max="4" width="92.375" customWidth="1"/>
     <col min="5" max="5" width="49.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -1096,7 +1108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>55</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>58</v>
       </c>
@@ -1138,14 +1150,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="92.4140625" customWidth="1"/>
+    <col min="2" max="2" width="25.875" customWidth="1"/>
+    <col min="4" max="4" width="92.375" customWidth="1"/>
     <col min="5" max="5" width="49.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>36</v>
       </c>
@@ -1167,7 +1179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>40</v>
       </c>

</xml_diff>